<commit_message>
Modify categories for section 19
</commit_message>
<xml_diff>
--- a/analysis_output.xlsx
+++ b/analysis_output.xlsx
@@ -3221,7 +3221,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3249,37 +3249,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Portals - MAC+ / TAP / USB / FAS</t>
+          <t>MAC+</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2283</v>
+        <v>1708</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>66.9%</t>
+          <t>50.1%</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Public Safety - LMS / GIFR / GEARS / CORE PATHWAY</t>
+          <t>TAP</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>292</v>
+        <v>407</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>8.6%</t>
+          <t>11.9%</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Gifted - MGI</t>
+          <t>MGI</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -3294,15 +3294,150 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>GIFR</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>132</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>3.9%</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>USB</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>128</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>3.8%</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>GEARS</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>107</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>3.1%</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>LMS</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>47</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1.4%</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>FAS</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>40</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1.2%</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>CORE PATHWAY</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>6</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0.2%</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>RLH Online</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Online Storefront (Shopify)</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>API Integration (Janus)</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>2872</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>84.2%</t>
+      <c r="B14" t="n">
+        <v>2874</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>84.3%</t>
         </is>
       </c>
     </row>
@@ -5392,7 +5527,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5420,37 +5555,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Portals - MAC+ / TAP / USB / FAS</t>
+          <t>MAC+</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>315</v>
+        <v>203</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>9.2%</t>
+          <t>6.0%</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Public Safety - LMS / GIFR / GEARS / CORE PATHWAY</t>
+          <t>TAP</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.2%</t>
+          <t>3.0%</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Gifted - MGI</t>
+          <t>MGI</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -5465,13 +5600,148 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>GIFR</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>USB</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0.2%</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>GEARS</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>LMS</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0.1%</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>FAS</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0.1%</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>CORE PATHWAY</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0.1%</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>RLH Online</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Online Storefront (Shopify)</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>API Integration (Janus)</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B14" t="n">
         <v>436</v>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>12.8%</t>
         </is>

</xml_diff>